<commit_message>
Implemented feature to send emails to addresses stored in an Excel file
</commit_message>
<xml_diff>
--- a/App-7-Automated-Emails/people.xlsx
+++ b/App-7-Automated-Emails/people.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Udemy\AdvancedPythonCourse\App-7-Automated-Emails\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD30530-6722-46C1-9E6F-F26998BF06A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -31,32 +40,10 @@
     <t>Smith</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>ypddjuio@yomail.info</t>
-    </r>
-  </si>
-  <si>
     <t>meditation</t>
   </si>
   <si>
     <t>Marry</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>kawnlyiw@supere.ml</t>
-    </r>
   </si>
   <si>
     <t>nasa</t>
@@ -68,50 +55,38 @@
     <t>Kann</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>pythonprocourse2@gmail.com</t>
-    </r>
+    <t>mvtukafke@emlhub.com</t>
+  </si>
+  <si>
+    <t>bhlrhpdl@drope.ml</t>
+  </si>
+  <si>
+    <t>ejwmipdl@drope.ml</t>
+  </si>
+  <si>
+    <t>football</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color theme="10"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -355,100 +330,166 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -650,7 +691,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -669,7 +710,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -699,7 +740,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -725,7 +766,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -751,7 +792,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -777,7 +818,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -803,7 +844,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -829,7 +870,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -855,7 +896,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -881,7 +922,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -907,7 +948,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,9 +961,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -939,7 +986,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -958,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -984,7 +1031,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1010,7 +1057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1036,7 +1083,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,7 +1109,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1088,7 +1135,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +1161,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1140,7 +1187,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1166,7 +1213,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1192,7 +1239,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1205,9 +1252,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1221,7 +1274,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1240,7 +1293,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1270,7 +1323,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,7 +1349,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1322,7 +1375,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1348,7 +1401,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1374,7 +1427,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1400,7 +1453,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1426,7 +1479,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1452,7 +1505,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1531,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1491,131 +1544,138 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.35156" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.35156" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s" s="6">
-        <v>7</v>
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="8">
-        <v>8</v>
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
       </c>
-      <c r="B3" t="s" s="9">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="10">
-        <v>9</v>
+      <c r="C3" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="D3" t="s" s="10">
-        <v>10</v>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>11</v>
+    <row r="4" spans="1:5" ht="14.7" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
       </c>
-      <c r="B4" t="s" s="9">
-        <v>12</v>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="10">
-        <v>10</v>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" ht="14.7" customHeight="1">
+    <row r="5" spans="1:5" ht="14.7" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" ht="14.7" customHeight="1">
+    <row r="6" spans="1:5" ht="14.7" customHeight="1">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" ht="14.7" customHeight="1">
+    <row r="7" spans="1:5" ht="14.7" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" ht="14.7" customHeight="1">
+    <row r="8" spans="1:5" ht="14.7" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" ht="14.7" customHeight="1">
+    <row r="9" spans="1:5" ht="14.7" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" ht="14.7" customHeight="1">
+    <row r="10" spans="1:5" ht="14.7" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -1624,12 +1684,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="ypddjuio@yomail.info"/>
-    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="kawnlyiw@supere.ml"/>
-    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display="pythonprocourse2@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>